<commit_message>
Made changes to the data codebook
</commit_message>
<xml_diff>
--- a/data/codebook/codebook.xlsx
+++ b/data/codebook/codebook.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhdan\minerva\Data science for social good\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1A1480-F90F-4D8E-B923-50BAD5BDF84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6B821C-4D4F-4DDF-BF3D-0D74AB52F377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{4DF23DC9-BFCA-42DB-9D36-6A6334B7469A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{4DF23DC9-BFCA-42DB-9D36-6A6334B7469A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Original dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Processed dataset" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="153">
   <si>
     <t>IL181 Gender inequality in online marketplaces</t>
   </si>
@@ -304,12 +304,6 @@
     <t>Some users have badges they have earned on the platform listed next to their username on their profile. These indicate whether they have been verified, have some kind of professional membership, amongst others. N/A indicates the user does not have the badge listed on their profile.</t>
   </si>
   <si>
-    <t>join_date_since_est</t>
-  </si>
-  <si>
-    <t>The date the user joined the Freelancer.com platform, represented as the number of days after the founding of Freelancer.com. For example, a value of "10" indicates the user joined 10 days after Freelancer.com was founded.</t>
-  </si>
-  <si>
     <t>Search query</t>
   </si>
   <si>
@@ -320,6 +314,186 @@
   </si>
   <si>
     <t>User inputted</t>
+  </si>
+  <si>
+    <t>join_date_from_earliest</t>
+  </si>
+  <si>
+    <t>The date the user joined the Freelancer.com platform, represented as the number of days after the earliest date in the dataset. For example, a value of "10" indicates the user joined 10 days after the earliest join date in the dataset. The earliest join date has a value of 0.</t>
+  </si>
+  <si>
+    <t>Codebook description:</t>
+  </si>
+  <si>
+    <t>This codebook is meant for the "original" version of the dataset before any matching-specific preprocessing occurred. The data file corresponding to this version of the codebook is "cleaned-gender-annotated-v5.csv".</t>
+  </si>
+  <si>
+    <t>This codebook corresponds to the dataset after matching-specific preprocessing was carried out. Many of the variables are now bucketed, and some have been condensed into new features that are derived from others. This version of the dataset is the one that was used for matching. The corresponding data file is "skills_certifications_categorized_female_treatment.csv".</t>
+  </si>
+  <si>
+    <t>The search query that was used to retrieve the user profile. For example, "software engineer" or "copywriter". This is kept only for reference, as the Freelancer search feature isn't that great. Do not use this value as an occupation indicator.</t>
+  </si>
+  <si>
+    <t>The name of the person. Only the first name is provided.</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Derived</t>
+  </si>
+  <si>
+    <t>The gender of the person -- can be "male" or "female". Male = 0, female = 1.</t>
+  </si>
+  <si>
+    <t>Location size</t>
+  </si>
+  <si>
+    <t>location_size</t>
+  </si>
+  <si>
+    <t>The size of the location where the user is based, with size being judged by the population of the place. 0 = extra small (smallest), 5 = extra extra large (biggest).</t>
+  </si>
+  <si>
+    <t>Engineering skills</t>
+  </si>
+  <si>
+    <t>engineering_skills</t>
+  </si>
+  <si>
+    <t>The number of engineering skills listed on a user's profile.</t>
+  </si>
+  <si>
+    <t>Writing skills</t>
+  </si>
+  <si>
+    <t>writing_skills</t>
+  </si>
+  <si>
+    <t>The number of writing skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Technical programming skills</t>
+  </si>
+  <si>
+    <t>technical_programming_skills</t>
+  </si>
+  <si>
+    <t>The number of technical programming skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Language translation skills</t>
+  </si>
+  <si>
+    <t>language_translation_skills</t>
+  </si>
+  <si>
+    <t>The number of language translation skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Finance and accounting skills</t>
+  </si>
+  <si>
+    <t>finance_accounting_skills</t>
+  </si>
+  <si>
+    <t>The number of finance and accounting skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Management skills</t>
+  </si>
+  <si>
+    <t>management_skills</t>
+  </si>
+  <si>
+    <t>The number of management skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Marketing and business skills</t>
+  </si>
+  <si>
+    <t>marketing_business_skills</t>
+  </si>
+  <si>
+    <t>The number of marketing and business skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Performance arts skills</t>
+  </si>
+  <si>
+    <t>performance_arts_skills</t>
+  </si>
+  <si>
+    <t>The number of performance arts skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Design skills</t>
+  </si>
+  <si>
+    <t>design_skills</t>
+  </si>
+  <si>
+    <t>The number of design skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Teaching and training skills</t>
+  </si>
+  <si>
+    <t>teaching_training_skills</t>
+  </si>
+  <si>
+    <t>The number of teaching and training skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Miscellaneous skills</t>
+  </si>
+  <si>
+    <t>miscellaneous_skills</t>
+  </si>
+  <si>
+    <t>The number of miscellaneous skills listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Language certifications</t>
+  </si>
+  <si>
+    <t>language_certifications</t>
+  </si>
+  <si>
+    <t>The number of language certifications listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Freelancer certifications</t>
+  </si>
+  <si>
+    <t>freelancer_certifications</t>
+  </si>
+  <si>
+    <t>The number of freelancer certifications listed on a user's profile</t>
+  </si>
+  <si>
+    <t>General skill certifications</t>
+  </si>
+  <si>
+    <t>general_skill_certifications</t>
+  </si>
+  <si>
+    <t>The number of general skill certifications listed on a user's profile</t>
+  </si>
+  <si>
+    <t>Programming certifications</t>
+  </si>
+  <si>
+    <t>programming_certifications</t>
+  </si>
+  <si>
+    <t>The number of programming certifications listed on a user's profile</t>
   </si>
 </sst>
 </file>
@@ -391,7 +565,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -408,8 +582,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -726,10 +907,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA575B06-5F6B-4D41-98A3-EF3AA7241F9B}">
-  <dimension ref="A2:H35"/>
+  <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.7" x14ac:dyDescent="0.45"/>
@@ -745,23 +926,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
@@ -771,122 +952,106 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B8" s="4" t="s">
+    <row r="7" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+      <c r="B8" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B10" s="5" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="35.1" x14ac:dyDescent="0.45">
-      <c r="B11" s="8" t="s">
+    <row r="13" spans="1:8" ht="35.1" x14ac:dyDescent="0.45">
+      <c r="B13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="E13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="35.1" x14ac:dyDescent="0.45">
-      <c r="B12" s="8" t="s">
+      <c r="G13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="35.1" x14ac:dyDescent="0.45">
+      <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>20</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>8</v>
@@ -898,18 +1063,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>17</v>
@@ -920,13 +1085,13 @@
     </row>
     <row r="16" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>8</v>
@@ -938,18 +1103,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="70.2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" ht="46.8" x14ac:dyDescent="0.45">
       <c r="B17" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>17</v>
@@ -960,16 +1125,16 @@
     </row>
     <row r="18" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B18" s="8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>17</v>
@@ -978,15 +1143,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:7" ht="70.2" x14ac:dyDescent="0.45">
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>32</v>
@@ -998,15 +1163,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="58.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B20" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>32</v>
@@ -1018,15 +1183,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:7" ht="46.8" x14ac:dyDescent="0.45">
       <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>32</v>
@@ -1038,15 +1203,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:7" ht="58.5" x14ac:dyDescent="0.45">
       <c r="B22" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>32</v>
@@ -1060,13 +1225,13 @@
     </row>
     <row r="23" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B23" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>32</v>
@@ -1075,18 +1240,18 @@
         <v>17</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B24" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>32</v>
@@ -1095,18 +1260,18 @@
         <v>17</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>82</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B25" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>32</v>
@@ -1120,13 +1285,13 @@
     </row>
     <row r="26" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>32</v>
@@ -1138,55 +1303,55 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>60</v>
+        <v>51</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>9</v>
+        <v>53</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B28" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="46.8" x14ac:dyDescent="0.45">
       <c r="B29" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>61</v>
@@ -1198,15 +1363,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
       <c r="B30" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>61</v>
@@ -1220,13 +1385,13 @@
     </row>
     <row r="31" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B31" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>61</v>
@@ -1240,13 +1405,13 @@
     </row>
     <row r="32" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B32" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>61</v>
@@ -1258,58 +1423,58 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="93.6" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B33" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B34" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="B35" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C35" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E35" s="8" t="s">
         <v>32</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="70.2" x14ac:dyDescent="0.45">
-      <c r="B34" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="81.900000000000006" x14ac:dyDescent="0.45">
-      <c r="B35" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>17</v>
@@ -1318,12 +1483,904 @@
         <v>82</v>
       </c>
     </row>
+    <row r="36" spans="2:7" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="B36" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="81.900000000000006" x14ac:dyDescent="0.45">
+      <c r="B37" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B8:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073704DE-84DF-4D33-AD34-8D8A23AF9554}">
+  <dimension ref="A2:H48"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.7" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.83984375" style="1"/>
+    <col min="2" max="2" width="16.578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1015625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.68359375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="2"/>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="2"/>
+      <c r="B6" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" ht="12.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="2"/>
+      <c r="B7" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" ht="64.2" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="2"/>
+      <c r="B8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B10" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="B13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B15" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="B16" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="B17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="B19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="58.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
+      <c r="B22" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B23" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
+      <c r="B24" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B25" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
+      <c r="B26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="46.8" x14ac:dyDescent="0.45">
+      <c r="B27" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="35.1" x14ac:dyDescent="0.45">
+      <c r="B28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B29" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B30" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B31" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B32" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="81.900000000000006" x14ac:dyDescent="0.45">
+      <c r="B33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B34" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B35" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B36" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B37" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B38" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B39" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B40" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B41" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B42" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B43" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B44" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B45" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B46" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B47" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B48" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>